<commit_message>
add res boundary attack for SEED 888
</commit_message>
<xml_diff>
--- a/results/SEED_888/result.xlsx
+++ b/results/SEED_888/result.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR12"/>
+  <dimension ref="A1:AZ12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,6 +558,18 @@
       <c r="AP1" s="1" t="n"/>
       <c r="AQ1" s="1" t="n"/>
       <c r="AR1" s="1" t="n"/>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>BOUNDARY</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="n"/>
+      <c r="AU1" s="1" t="n"/>
+      <c r="AV1" s="1" t="n"/>
+      <c r="AW1" s="1" t="n"/>
+      <c r="AX1" s="1" t="n"/>
+      <c r="AY1" s="1" t="n"/>
+      <c r="AZ1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="B2" s="1" t="inlineStr">
@@ -775,6 +787,46 @@
           <t>0.20</t>
         </is>
       </c>
+      <c r="AS2" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="AT2" s="1" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="AU2" s="1" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="AV2" s="1" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
+      <c r="AW2" s="1" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="AX2" s="1" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="AY2" s="1" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="AZ2" s="1" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -924,6 +976,30 @@
       </c>
       <c r="AR4" t="n">
         <v>31.47039794921875</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>4.225946426391602</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>4.250112533569336</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>4.336052894592285</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>4.419761180877686</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>4.485738754272461</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>4.650653839111328</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>4.967658996582031</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>6.78828239440918</v>
       </c>
     </row>
     <row r="5">
@@ -1059,6 +1135,30 @@
       <c r="AR5" t="n">
         <v>31.70050949505534</v>
       </c>
+      <c r="AS5" t="n">
+        <v>5.380455087749915</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>5.393753691812359</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>5.469000935928117</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>5.600021512126475</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>5.667467995626028</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>5.902176678537989</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>6.213391626491155</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>8.565021227238546</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
@@ -1193,6 +1293,30 @@
       <c r="AR6" t="n">
         <v>0.9843993186950684</v>
       </c>
+      <c r="AS6" t="n">
+        <v>0.9996083378791809</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.9996046423912048</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.9995924234390259</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>0.9995657205581665</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>0.9995605945587158</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>0.9995237588882446</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>0.9994716048240662</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>0.9989577531814575</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1330,6 +1454,30 @@
       </c>
       <c r="AR7" t="n">
         <v>37.08818054199219</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>2.530349493026733</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>2.62942099571228</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>3.02424693107605</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>3.525465488433838</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>3.796053171157837</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>5.369766712188721</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>6.114477157592773</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>11.37678623199463</v>
       </c>
     </row>
     <row r="8">
@@ -1465,6 +1613,30 @@
       <c r="AR8" t="n">
         <v>37.34682093806229</v>
       </c>
+      <c r="AS8" t="n">
+        <v>3.397235385900117</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>3.526560547523482</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>3.989035360421044</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>4.516633551406989</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>4.837836809286371</v>
+      </c>
+      <c r="AX8" t="n">
+        <v>6.799186927206351</v>
+      </c>
+      <c r="AY8" t="n">
+        <v>7.795911343332202</v>
+      </c>
+      <c r="AZ8" t="n">
+        <v>14.370735929223</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
@@ -1599,6 +1771,30 @@
       <c r="AR9" t="n">
         <v>0.9749844670295715</v>
       </c>
+      <c r="AS9" t="n">
+        <v>0.9997932910919189</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0.9997768998146057</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0.9997138977050781</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>0.999633252620697</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>0.9995796084403992</v>
+      </c>
+      <c r="AX9" t="n">
+        <v>0.9991684556007385</v>
+      </c>
+      <c r="AY9" t="n">
+        <v>0.998913049697876</v>
+      </c>
+      <c r="AZ9" t="n">
+        <v>0.9962786436080933</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1736,6 +1932,30 @@
       </c>
       <c r="AR10" t="n">
         <v>30.26678276062012</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>2.684278964996338</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>2.818708896636963</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>3.036305904388428</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>3.248105525970459</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>3.627833604812622</v>
+      </c>
+      <c r="AX10" t="n">
+        <v>4.270208358764648</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>5.393082141876221</v>
+      </c>
+      <c r="AZ10" t="n">
+        <v>9.396393775939941</v>
       </c>
     </row>
     <row r="11">
@@ -1871,6 +2091,30 @@
       <c r="AR11" t="n">
         <v>30.48255196208306</v>
       </c>
+      <c r="AS11" t="n">
+        <v>3.573498128986309</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>3.72261359559607</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>3.946034220033302</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>4.187992123965315</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>4.542967700384122</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>5.41309853431355</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>6.670052558657534</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>11.65110423867492</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
@@ -2005,9 +2249,33 @@
       <c r="AR12" t="n">
         <v>0.9833714365959167</v>
       </c>
+      <c r="AS12" t="n">
+        <v>0.9997835159301758</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0.9997653365135193</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0.9997282028198242</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>0.9996936321258545</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>0.9996384978294373</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>0.9994862079620361</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>0.9992225766181946</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>0.9976072311401367</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="M1:T1"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A9"/>
@@ -2016,6 +2284,7 @@
     <mergeCell ref="AC1:AJ1"/>
     <mergeCell ref="AK1:AR1"/>
     <mergeCell ref="U1:AB1"/>
+    <mergeCell ref="AS1:AZ1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>